<commit_message>
update example data covariates for FUN MP
</commit_message>
<xml_diff>
--- a/braph2genesis/pipelines/functional multiplex/example data FUN_MP (fMRI)/xls/GroupName1/GroupName1_covariates.xlsx
+++ b/braph2genesis/pipelines/functional multiplex/example data FUN_MP (fMRI)/xls/GroupName1/GroupName1_covariates.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -229,6 +229,33 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
   <si>
     <t>edu</t>
@@ -280,10 +307,10 @@
   <dimension ref="A1:D51"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="true"/>
-    <col min="2" max="2" width="4.28515625" customWidth="true"/>
-    <col min="3" max="3" width="7.7109375" customWidth="true"/>
-    <col min="4" max="4" width="4.5703125" customWidth="true"/>
+    <col min="1" max="1" width="9.07421875" customWidth="true"/>
+    <col min="2" max="2" width="4.07421875" customWidth="true"/>
+    <col min="3" max="3" width="7.16796875" customWidth="true"/>
+    <col min="4" max="4" width="4.34765625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -297,7 +324,7 @@
         <v>52</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
@@ -305,13 +332,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>53</v>
       </c>
       <c r="D2" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -319,13 +346,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -333,13 +360,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="0">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -347,13 +374,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -361,13 +388,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="0">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -375,13 +402,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="0">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -389,13 +416,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -403,13 +430,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D9" s="0">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -417,10 +444,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10" s="0">
         <v>5</v>
@@ -431,13 +458,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="0">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -445,13 +472,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D12" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -459,13 +486,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="0">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
@@ -473,13 +500,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D14" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -487,13 +514,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D15" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -501,13 +528,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16" s="0">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -515,13 +542,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17" s="0">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -529,13 +556,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="0">
+        <v>68</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="D18" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -543,13 +570,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="0">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D19" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
@@ -557,10 +584,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="0">
+        <v>74</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="D20" s="0">
         <v>5</v>
@@ -571,13 +598,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="0">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
@@ -585,10 +612,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="0">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" s="0">
         <v>7</v>
@@ -599,13 +626,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="0">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D23" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -613,13 +640,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="0">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D24" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
@@ -627,13 +654,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="0">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" s="0">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26">
@@ -641,10 +668,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="0">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D26" s="0">
         <v>9</v>
@@ -655,13 +682,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="0">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D27" s="0">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28">
@@ -669,13 +696,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="0">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D28" s="0">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
@@ -683,13 +710,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="0">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D29" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
@@ -697,13 +724,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="0">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D30" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
@@ -711,13 +738,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="0">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D31" s="0">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
@@ -725,13 +752,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="0">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D32" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33">
@@ -739,13 +766,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="0">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D33" s="0">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -753,13 +780,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="0">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D34" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
@@ -767,13 +794,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="0">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D35" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36">
@@ -781,13 +808,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="0">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D36" s="0">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37">
@@ -795,13 +822,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="0">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D37" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
@@ -809,13 +836,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="0">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D38" s="0">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
@@ -823,13 +850,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="0">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D39" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
@@ -837,13 +864,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="0">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D40" s="0">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41">
@@ -851,13 +878,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="0">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D41" s="0">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
@@ -865,13 +892,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="0">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D42" s="0">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43">
@@ -879,13 +906,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="0">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D43" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
@@ -893,13 +920,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="0">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D44" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45">
@@ -907,13 +934,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="0">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D45" s="0">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46">
@@ -921,13 +948,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="0">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D46" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
@@ -935,13 +962,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="0">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D47" s="0">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48">
@@ -949,13 +976,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="0">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D48" s="0">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49">
@@ -963,13 +990,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="0">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D49" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50">
@@ -977,13 +1004,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="0">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D50" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
@@ -991,13 +1018,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="0">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D51" s="0">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>